<commit_message>
building failsafes on input e processing
</commit_message>
<xml_diff>
--- a/test_contacts.xlsx
+++ b/test_contacts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,70 +436,122 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>paciente</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>phone</t>
+          <t>tel.recado</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>tel.celular</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>message</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>data.solicitacao</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>diagnostico</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>John Doe</t>
+          <t>João Silva</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+1234567890</t>
+          <t>11 - 9999 - 9999</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Hello John!</t>
-        </is>
-      </c>
+          <t>11 - 8888 - 8888</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Olá João! Lembrete de consulta.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Jane Smith</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>+0987654321</t>
+          <t>11 - 9999 - 9999</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Hi Jane!</t>
-        </is>
-      </c>
+          <t>11 - 8888 - 8888</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Olá Lembrete de consulta.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>29/08/2025</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bob Wilson</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>+1112223333</t>
-        </is>
-      </c>
+          <t>Maria Santos</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Hey Bob!</t>
-        </is>
-      </c>
+          <t>11 - 7777 - 7777</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Olá Maria! Confirmação de horário.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>cirurgia</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Silva</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Olá Silva! Lembrete de consulta.</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>